<commit_message>
fix: openpyxl.to_df to handle no headers better
</commit_message>
<xml_diff>
--- a/tests/io/data/multi_index.xlsx
+++ b/tests/io/data/multi_index.xlsx
@@ -1,31 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alee7/ucsf/git/macpie/tests/io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A671D223-742E-354A-9B64-1A3F2677473C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB89B9E-B05F-384A-B66E-59BCB71C1CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="-18820" windowWidth="29660" windowHeight="18080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34760" yWindow="820" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="0_0" sheetId="1" r:id="rId1"/>
-    <sheet name="1_0" sheetId="2" r:id="rId2"/>
-    <sheet name="0_1" sheetId="6" r:id="rId3"/>
-    <sheet name="1_1" sheetId="3" r:id="rId4"/>
+    <sheet name="1_0" sheetId="2" r:id="rId1"/>
+    <sheet name="1_1" sheetId="3" r:id="rId2"/>
+    <sheet name="1_2" sheetId="9" r:id="rId3"/>
+    <sheet name="2_0" sheetId="8" r:id="rId4"/>
     <sheet name="2_1" sheetId="4" r:id="rId5"/>
     <sheet name="2_2" sheetId="5" r:id="rId6"/>
+    <sheet name="0_0" sheetId="1" r:id="rId7"/>
+    <sheet name="0_1" sheetId="6" r:id="rId8"/>
+    <sheet name="0_2" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="31">
   <si>
     <t>PIDN</t>
   </si>
@@ -460,175 +463,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1">
-        <v>43831</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>9</v>
-      </c>
-      <c r="H1">
-        <v>9</v>
-      </c>
-      <c r="I1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43831</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43831</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>8</v>
-      </c>
-      <c r="I3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43831</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>9</v>
-      </c>
-      <c r="I4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43831</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD35D5E-CF81-894A-9299-B696183C3963}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -824,198 +658,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA708C40-7C28-EF4B-A867-1518E117AC0D}">
-  <dimension ref="A1:J5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1">
-        <v>43831</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>9</v>
-      </c>
-      <c r="I1">
-        <v>9</v>
-      </c>
-      <c r="J1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1">
-        <v>43831</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1">
-        <v>43831</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1">
-        <v>43831</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>9</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1">
-        <v>43831</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>10</v>
-      </c>
-      <c r="J5">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165DB06F-FC79-7341-B597-DE714BFBD198}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1222,13 +869,462 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E423E685-3FDF-BD44-AB94-2A6E13F06848}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C63C95-64A0-A445-AF06-72DE91FD07A4}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DEE255D-992C-D64F-B7CB-AAA920BD7089}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1717,4 +1813,551 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>9</v>
+      </c>
+      <c r="H1">
+        <v>9</v>
+      </c>
+      <c r="I1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>43831</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA708C40-7C28-EF4B-A867-1518E117AC0D}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1">
+        <v>43831</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>9</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43831</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43831</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1">
+        <v>43831</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66533431-486F-7D46-96A7-0DFA5E6F40A6}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+      <c r="K4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>43831</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>